<commit_message>
now with 2 piecharts
</commit_message>
<xml_diff>
--- a/documentation/import_samples/2025-04-01-2025-06-30 Excel File.xlsx
+++ b/documentation/import_samples/2025-04-01-2025-06-30 Excel File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WimpieProgramming\DCIPythonCourse\FinalProject\FamilyThings\documentation\import_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EADE818-B137-41C3-8EDD-148AF54699CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3678530B-1EDD-4950-BE1A-9E71B4A897E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FA4BD02-AD15-42C5-9862-36D11F910600}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FA4BD02-AD15-42C5-9862-36D11F910600}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1688,7 +1688,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1706,7 +1706,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3039,7 +3038,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{45FEB23A-A7B3-4458-AAB7-7B1DDFDA6577}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{45FEB23A-A7B3-4458-AAB7-7B1DDFDA6577}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B38" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -3555,7 +3554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6755,7 +6754,7 @@
       <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2">
         <v>-33.47</v>
       </c>
     </row>
@@ -6763,7 +6762,7 @@
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3">
         <v>-4.9000000000000004</v>
       </c>
     </row>
@@ -6771,7 +6770,7 @@
       <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4">
         <v>-452.47</v>
       </c>
     </row>
@@ -6779,7 +6778,7 @@
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5">
         <v>-36.93</v>
       </c>
     </row>
@@ -6787,7 +6786,7 @@
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6">
         <v>-84.56</v>
       </c>
     </row>
@@ -6795,7 +6794,7 @@
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7">
         <v>-77</v>
       </c>
     </row>
@@ -6803,7 +6802,7 @@
       <c r="A8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8">
         <v>-2.5</v>
       </c>
     </row>
@@ -6811,7 +6810,7 @@
       <c r="A9" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9">
         <v>-45.16</v>
       </c>
     </row>
@@ -6819,7 +6818,7 @@
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10">
         <v>765</v>
       </c>
     </row>
@@ -6827,7 +6826,7 @@
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11">
         <v>4500</v>
       </c>
     </row>
@@ -6835,7 +6834,7 @@
       <c r="A12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12">
         <v>-450</v>
       </c>
     </row>
@@ -6843,7 +6842,7 @@
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13">
         <v>-135.75</v>
       </c>
     </row>
@@ -6851,7 +6850,7 @@
       <c r="A14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14">
         <v>280.22000000000003</v>
       </c>
     </row>
@@ -6859,7 +6858,7 @@
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15">
         <v>-44.97</v>
       </c>
     </row>
@@ -6867,7 +6866,7 @@
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16">
         <v>-65.36</v>
       </c>
     </row>
@@ -6875,7 +6874,7 @@
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17">
         <v>-72</v>
       </c>
     </row>
@@ -6883,7 +6882,7 @@
       <c r="A18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18">
         <v>-325</v>
       </c>
     </row>
@@ -6891,7 +6890,7 @@
       <c r="A19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19">
         <v>-66.099999999999994</v>
       </c>
     </row>
@@ -6899,7 +6898,7 @@
       <c r="A20" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20">
         <v>-848.6099999999999</v>
       </c>
     </row>
@@ -6907,7 +6906,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21">
         <v>-289.29000000000002</v>
       </c>
     </row>
@@ -6915,7 +6914,7 @@
       <c r="A22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22">
         <v>-56.17</v>
       </c>
     </row>
@@ -6923,7 +6922,7 @@
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23">
         <v>-50</v>
       </c>
     </row>
@@ -6931,7 +6930,7 @@
       <c r="A24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24">
         <v>-97.51</v>
       </c>
     </row>
@@ -6939,7 +6938,7 @@
       <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25">
         <v>-400.53000000000009</v>
       </c>
     </row>
@@ -6947,7 +6946,7 @@
       <c r="A26" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26">
         <v>-83.14</v>
       </c>
     </row>
@@ -6955,7 +6954,7 @@
       <c r="A27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27">
         <v>-20.98</v>
       </c>
     </row>
@@ -6963,7 +6962,7 @@
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28">
         <v>-23.49</v>
       </c>
     </row>
@@ -6971,7 +6970,7 @@
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29">
         <v>-55.08</v>
       </c>
     </row>
@@ -6979,7 +6978,7 @@
       <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30">
         <v>-263.26</v>
       </c>
     </row>
@@ -6987,7 +6986,7 @@
       <c r="A31" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31">
         <v>-9.39</v>
       </c>
     </row>
@@ -6995,7 +6994,7 @@
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32">
         <v>-142.62</v>
       </c>
     </row>
@@ -7003,7 +7002,7 @@
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33">
         <v>-107.29</v>
       </c>
     </row>
@@ -7011,7 +7010,7 @@
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34">
         <v>-7</v>
       </c>
     </row>
@@ -7019,7 +7018,7 @@
       <c r="A35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35">
         <v>-71.599999999999994</v>
       </c>
     </row>
@@ -7027,7 +7026,7 @@
       <c r="A36" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36">
         <v>-101.36</v>
       </c>
     </row>
@@ -7035,7 +7034,7 @@
       <c r="A37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37">
         <v>-22</v>
       </c>
     </row>
@@ -7043,7 +7042,7 @@
       <c r="A38" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38">
         <v>999.73000000000013</v>
       </c>
     </row>

</xml_diff>